<commit_message>
bug fix on time series writing
- to do -> a mapping of tyndp 2024 nodes and res time series node needed as input for the '''construct_data_dictionary_2024''' function
</commit_message>
<xml_diff>
--- a/data_sources/TYNDP2024/LIST OF NODES_2024.xlsx
+++ b/data_sources/TYNDP2024/LIST OF NODES_2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giacomobastianel/.julia/dev/EU_grid_operations/data_sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hergun/Julia files/EU_grid_operations/data_sources/TYNDP2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111B8B95-738D-8E46-B18C-5C05822A1F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E370005B-A5A0-CD43-A17E-5DA224F864A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{01EDC9EF-BF44-4FD4-BE0A-DC4E630D6F16}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{01EDC9EF-BF44-4FD4-BE0A-DC4E630D6F16}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity" sheetId="1" r:id="rId1"/>
@@ -1164,12 +1164,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E6A4E6-5176-4037-BD12-E7E86AE4E35B}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:XFD70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3814,11 +3815,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <MYENTSOE_SiteType xmlns="9b216c6c-829b-4bd6-a7b8-61d756915eca">MYENTSOE</MYENTSOE_SiteType>
@@ -3870,6 +3866,11 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A42DABF1-2B9A-4CA1-8B81-2951C1872D30}">
   <ds:schemaRefs>
@@ -3890,14 +3891,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A85D3267-1197-4C47-A194-F537B10B8D80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E5ECECB-61BB-479C-90F6-8F41879C55DB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3906,4 +3899,12 @@
     <ds:schemaRef ds:uri="e3fb2008-9808-4f29-aa32-2f66631018ed"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A85D3267-1197-4C47-A194-F537B10B8D80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>